<commit_message>
'Fixing an error with chisquare test in Data exploraion section. Test run from scipy package was done on a wrong sample - categorical data were normalized, while it shouldn't.
</commit_message>
<xml_diff>
--- a/data/chisquare.xlsx
+++ b/data/chisquare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\What_makes_cell_alive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Piotrek\Hidden_in_genes\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25692373-DE32-4107-A69C-EF746BF74F58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A10CE34-9FAC-4B89-9650-DAEA3BA1E2FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="610" yWindow="1170" windowWidth="10760" windowHeight="7040" xr2:uid="{E63685CA-3A48-4A8F-9472-44889F91D50C}"/>
+    <workbookView xWindow="3130" yWindow="1630" windowWidth="12940" windowHeight="7240" xr2:uid="{E63685CA-3A48-4A8F-9472-44889F91D50C}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,13 @@
     <t>GC content below \n length below</t>
   </si>
   <si>
-    <t>GC content below \n lenght above</t>
-  </si>
-  <si>
     <t>GC content above \n length below</t>
   </si>
   <si>
-    <t>GC content above \n lenght above</t>
+    <t>GC content above \n length above</t>
+  </si>
+  <si>
+    <t>GC content below \n length above</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -487,15 +487,15 @@
       </c>
       <c r="G2" s="1">
         <f>SUM(F2:F5)</f>
-        <v>118.07872412623007</v>
+        <v>118.63522225992534</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>1675</v>
+        <v>1265</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C5" si="0">5894/4</f>
@@ -503,23 +503,23 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D5" si="1">B3-C3</f>
-        <v>201.5</v>
+        <v>-208.5</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E5" si="2">D3^2</f>
-        <v>40602.25</v>
+        <v>43472.25</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F5" si="3">E3/C3</f>
-        <v>27.554971157108923</v>
+        <v>29.502714625042415</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>1689</v>
+        <v>1676</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -527,23 +527,23 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>215.5</v>
+        <v>202.5</v>
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>46440.25</v>
+        <v>41006.25</v>
       </c>
       <c r="F4">
         <f t="shared" si="3"/>
-        <v>31.516966406515099</v>
+        <v>27.829148286392943</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>1266</v>
+        <v>1689</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -551,15 +551,15 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-207.5</v>
+        <v>215.5</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>43056.25</v>
+        <v>46440.25</v>
       </c>
       <c r="F5">
         <f t="shared" si="3"/>
-        <v>29.22039362063115</v>
+        <v>31.516966406515099</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -571,6 +571,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>